<commit_message>
updating excel files for easier processing
</commit_message>
<xml_diff>
--- a/sampleData/REF2021Results-SelectedSamples-resultsSummary.xlsx
+++ b/sampleData/REF2021Results-SelectedSamples-resultsSummary.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akj22/Dropbox/Kent/teaching/COMP6481/COMP6or8481 cw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akj22/PDocuments/workspace/git/COMP6481-8481/sampleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F9A779-42B9-C74B-B87B-F305DAC9B257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF29A115-8C9C-A745-8F17-4D6401536F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21760" yWindow="500" windowWidth="19720" windowHeight="20500" xr2:uid="{F77AB548-6C7B-4D93-8364-DE37B33C5798}"/>
+    <workbookView xWindow="13880" yWindow="500" windowWidth="19720" windowHeight="20500" xr2:uid="{F77AB548-6C7B-4D93-8364-DE37B33C5798}"/>
   </bookViews>
   <sheets>
-    <sheet name="SELECTION + explanation" sheetId="3" r:id="rId1"/>
-    <sheet name="selected all results" sheetId="2" r:id="rId2"/>
+    <sheet name="selected all results" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'selected all results'!$A$1:$O$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'selected all results'!$A$1:$O$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="42">
   <si>
     <t>Institution code (UKPRN)</t>
   </si>
@@ -160,92 +159,18 @@
     <t>weighted * score</t>
   </si>
   <si>
-    <t>environment better than Kent</t>
-  </si>
-  <si>
-    <t>environment worse than Kent</t>
-  </si>
-  <si>
-    <t>ave env deficit</t>
-  </si>
-  <si>
-    <t>ave env improvement</t>
-  </si>
-  <si>
     <t>diff from Kent</t>
   </si>
   <si>
     <t>Environment +-</t>
-  </si>
-  <si>
-    <t>Selection criteria</t>
-  </si>
-  <si>
-    <t>ENV better than Kent</t>
-  </si>
-  <si>
-    <t>outputs within 0.05 of Kent</t>
-  </si>
-  <si>
-    <t>both:</t>
-  </si>
-  <si>
-    <t>ENV worse than Kent</t>
-  </si>
-  <si>
-    <t>outputs within 0.25 of Kent</t>
-  </si>
-  <si>
-    <t>* observation: those with output scores close to Kent tended to do better overall in environment</t>
-  </si>
-  <si>
-    <t>size +- 25 of Kent FTE (full time equivalent, where a single full time employee is 1.0, and part time employees are a fraction of an FTE between 0 and 1 exclusive)</t>
-  </si>
-  <si>
-    <t>9 (10% of 90) selected to represent each set of samples, keeping similar distributions for better-than and worse-than samples</t>
-  </si>
-  <si>
-    <t>Scoring for REF2021</t>
-  </si>
-  <si>
-    <t>From https://ref.ac.uk/guidance-on-results/guidance-on-ref-2021-results/</t>
-  </si>
-  <si>
-    <t>Multiply 4* ratings by 4</t>
-  </si>
-  <si>
-    <t>Multiply 3* ratings by 1</t>
-  </si>
-  <si>
-    <t>Rationale behind weighted score:</t>
-  </si>
-  <si>
-    <t>(no income from these in REF2014)</t>
-  </si>
-  <si>
-    <t>(these contributed a small part of income in REF2014)</t>
-  </si>
-  <si>
-    <t>(these contributed the majority of income in REF2014)</t>
-  </si>
-  <si>
-    <t>Disregard 2*, 1*, unclassified entirely from score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -255,14 +180,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -314,20 +231,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -347,104 +255,20 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -477,72 +301,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Image showing the breakdown of the overall quality profile into its 3 components of outputs (60%), impact (25%) and environment (15%)">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84B99F2F-4E7E-68DB-2647-22CC98447BEA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="7239000"/>
-          <a:ext cx="8178800" cy="5359400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,371 +599,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BCBE44-F26A-994E-A6F0-4F78A1E28B01}">
-  <dimension ref="A1:C73"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0.40625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.40625</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="4">
-        <v>0.21875</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0.40625</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="10">
-        <f>AVERAGE(C13:C21)</f>
-        <v>0.3888888888888889</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="4">
-        <v>-0.46875</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="4">
-        <v>-0.1875</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="4">
-        <v>-0.375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="4">
-        <v>-0.46875</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="4">
-        <v>-0.375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="4">
-        <v>-0.5625</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="4">
-        <v>-0.5625</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="4">
-        <v>-0.5625</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="16">
-        <v>-0.375</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B34" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="12">
-        <f>AVERAGE(C25:C33)</f>
-        <v>-0.4375</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>57</v>
-      </c>
-      <c r="B71" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>58</v>
-      </c>
-      <c r="B72" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>63</v>
-      </c>
-      <c r="B73" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:C33">
-    <sortCondition ref="A25:A33"/>
-  </sortState>
-  <conditionalFormatting sqref="A12 A24">
-    <cfRule type="containsText" dxfId="11" priority="7" stopIfTrue="1" operator="containsText" text="WORSE">
-      <formula>NOT(ISERROR(SEARCH("WORSE",A12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" stopIfTrue="1" operator="containsText" text="BETTER">
-      <formula>NOT(ISERROR(SEARCH("BETTER",A12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21 B16:B19">
-    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="WORSE">
-      <formula>NOT(ISERROR(SEARCH("WORSE",B16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="BETTER">
-      <formula>NOT(ISERROR(SEARCH("BETTER",B16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B25:B33">
-    <cfRule type="containsText" dxfId="7" priority="3" stopIfTrue="1" operator="containsText" text="WORSE">
-      <formula>NOT(ISERROR(SEARCH("WORSE",B25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" stopIfTrue="1" operator="containsText" text="BETTER">
-      <formula>NOT(ISERROR(SEARCH("BETTER",B25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="WORSE">
-      <formula>NOT(ISERROR(SEARCH("WORSE",B15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" stopIfTrue="1" operator="containsText" text="BETTER">
-      <formula>NOT(ISERROR(SEARCH("BETTER",B15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A2F396-F4FB-1943-95EE-A54265D8E40F}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1228,7 +625,7 @@
         <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1257,11 +654,11 @@
       <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="13" t="s">
-        <v>44</v>
+      <c r="P1" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -5295,18 +4692,18 @@
   </sheetData>
   <autoFilter ref="A1:O77" xr:uid="{81A2F396-F4FB-1943-95EE-A54265D8E40F}"/>
   <conditionalFormatting sqref="D66:D77 D38:D61 D22:D33 D1:D9">
-    <cfRule type="containsText" dxfId="5" priority="9" stopIfTrue="1" operator="containsText" text="WORSE">
+    <cfRule type="containsText" dxfId="3" priority="9" stopIfTrue="1" operator="containsText" text="WORSE">
       <formula>NOT(ISERROR(SEARCH("WORSE",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" stopIfTrue="1" operator="containsText" text="BETTER">
+    <cfRule type="containsText" dxfId="2" priority="10" stopIfTrue="1" operator="containsText" text="BETTER">
       <formula>NOT(ISERROR(SEARCH("BETTER",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:N77">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$J2&lt;&gt;"Overall"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>$J2="Overall"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>